<commit_message>
Clean up and move to R:
</commit_message>
<xml_diff>
--- a/site/res/json/_Last-month-raceData.xlsx
+++ b/site/res/json/_Last-month-raceData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\frimleyFlyers\site\res\json\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\git\frimleyFlyers\site\res\json\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD2DB8D-2439-45D1-A028-848418AE1521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3719FFD-1DEB-4893-807A-05AA03066341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F8E35614-E497-4037-9098-C44996FE8116}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F8E35614-E497-4037-9098-C44996FE8116}"/>
   </bookViews>
   <sheets>
     <sheet name="b-raceData2024.json" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="73">
   <si>
     <t>Column1</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Pts</t>
   </si>
   <si>
-    <t>Alan Bush</t>
-  </si>
-  <si>
     <t>Susan Harvey</t>
   </si>
   <si>
@@ -76,159 +73,51 @@
     <t>Darren Stone</t>
   </si>
   <si>
-    <t>Simon Harvey</t>
-  </si>
-  <si>
-    <t>Andy Poulter</t>
-  </si>
-  <si>
     <t>James Ball</t>
   </si>
   <si>
     <t>Matthew Knight</t>
   </si>
   <si>
-    <t>Brooklands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22:36	</t>
-  </si>
-  <si>
     <t>Fiona Keane-Munday</t>
   </si>
   <si>
     <t>Hogmoor Inclosure</t>
   </si>
   <si>
-    <t>Chris Peddle</t>
-  </si>
-  <si>
     <t>Wendy Ockrim</t>
   </si>
   <si>
-    <t>Louise McIntosh</t>
-  </si>
-  <si>
     <t>Lucy Bass</t>
   </si>
   <si>
-    <t>Ben Gay</t>
-  </si>
-  <si>
     <t>Home</t>
   </si>
   <si>
-    <t xml:space="preserve">28:50	</t>
-  </si>
-  <si>
     <t>Jo Longmuir</t>
   </si>
   <si>
-    <t xml:space="preserve">23:03	</t>
-  </si>
-  <si>
     <t>Rebecca Williams</t>
   </si>
   <si>
-    <t xml:space="preserve">31:03	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22:01	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22:33	</t>
-  </si>
-  <si>
     <t>Charlotte Knight</t>
   </si>
   <si>
-    <t xml:space="preserve">34:51	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20:52	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34:22	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23:14	</t>
-  </si>
-  <si>
     <t>Jen Knight</t>
   </si>
   <si>
-    <t xml:space="preserve">35:34	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30:42	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22:17	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">41:27	</t>
-  </si>
-  <si>
     <t>Alasdair Nuttall</t>
   </si>
   <si>
-    <t xml:space="preserve">26:05	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29:57	</t>
-  </si>
-  <si>
     <t>Sarah Campbell-Foster</t>
   </si>
   <si>
-    <t xml:space="preserve">31:57	</t>
-  </si>
-  <si>
-    <t>Lewis Whatley</t>
-  </si>
-  <si>
-    <t>Basingstoke</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19:39	</t>
-  </si>
-  <si>
-    <t>Leonie Harvey</t>
-  </si>
-  <si>
-    <t>Frimley Lodge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27:59	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22:53	</t>
-  </si>
-  <si>
     <t>Kev Knight</t>
   </si>
   <si>
-    <t xml:space="preserve">25:46	</t>
-  </si>
-  <si>
-    <t>Karen Phillips</t>
-  </si>
-  <si>
-    <t>Cutler Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28:46	</t>
-  </si>
-  <si>
     <t>Ashton Peddle</t>
   </si>
   <si>
-    <t xml:space="preserve">37:05	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27:44	</t>
-  </si>
-  <si>
     <t xml:space="preserve">33:25	</t>
   </si>
   <si>
@@ -254,6 +143,102 @@
   </si>
   <si>
     <t xml:space="preserve">27:42	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29:20	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36:19	</t>
+  </si>
+  <si>
+    <t>Rushmoor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29:39	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21:20	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21:05	</t>
+  </si>
+  <si>
+    <t>Banbury</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24:05	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33:55	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30:20	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22:05	</t>
+  </si>
+  <si>
+    <t>Susan Rodrigues</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23:49	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35:36	</t>
+  </si>
+  <si>
+    <t>Tom Churchill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28:48	</t>
+  </si>
+  <si>
+    <t>Grove Fields</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27:01	</t>
+  </si>
+  <si>
+    <t>Martin Gay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26:53	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">38:04	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33:39	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34:11	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32:12	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35:06	</t>
+  </si>
+  <si>
+    <t>Edenbrook Country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33:35	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29:04	</t>
+  </si>
+  <si>
+    <t>Paul Bass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33:56	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">44:06	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35:35	</t>
   </si>
 </sst>
 </file>
@@ -1160,17 +1145,17 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1187,7 +1172,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -1204,423 +1189,423 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="D3" s="1">
-        <v>-8.2500000000000004E-2</v>
+        <v>-0.12570000000000001</v>
       </c>
       <c r="E3" s="2">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="D4" s="1">
-        <v>-6.59E-2</v>
+        <v>-7.5899999999999995E-2</v>
       </c>
       <c r="E4" s="2">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="D5" s="1">
-        <v>5.1000000000000004E-3</v>
+        <v>-3.8399999999999997E-2</v>
       </c>
       <c r="E5" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="D6" s="1">
-        <v>7.0000000000000001E-3</v>
+        <v>-1.61E-2</v>
       </c>
       <c r="E6" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D7" s="1">
-        <v>1.54E-2</v>
+        <v>9.5999999999999992E-3</v>
       </c>
       <c r="E7" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D8" s="1">
-        <v>3.3599999999999998E-2</v>
+        <v>2.4799999999999999E-2</v>
       </c>
       <c r="E8" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D9" s="1">
-        <v>3.8699999999999998E-2</v>
+        <v>3.1399999999999997E-2</v>
       </c>
       <c r="E9" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D10" s="1">
-        <v>3.9899999999999998E-2</v>
+        <v>3.5900000000000001E-2</v>
       </c>
       <c r="E10" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="D11" s="1">
-        <v>4.5100000000000001E-2</v>
+        <v>4.2500000000000003E-2</v>
       </c>
       <c r="E11" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="D12" s="1">
-        <v>4.58E-2</v>
+        <v>5.2299999999999999E-2</v>
       </c>
       <c r="E12" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D13" s="1">
-        <v>4.7100000000000003E-2</v>
+        <v>5.79E-2</v>
       </c>
       <c r="E13" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="D14" s="1">
-        <v>4.8399999999999999E-2</v>
+        <v>7.3300000000000004E-2</v>
       </c>
       <c r="E14" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="C15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="1">
+        <v>9.9699999999999997E-2</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="1">
-        <v>5.1900000000000002E-2</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="C17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.1207</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.13550000000000001</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0.13750000000000001</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" s="1">
-        <v>5.4699999999999999E-2</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="1">
-        <v>5.74E-2</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.14180000000000001</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.1527</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="1">
-        <v>6.2100000000000002E-2</v>
-      </c>
-      <c r="E18" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="1">
-        <v>7.8200000000000006E-2</v>
-      </c>
-      <c r="E19" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B20" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="1">
-        <v>8.2600000000000007E-2</v>
-      </c>
-      <c r="E20" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" s="1">
-        <v>8.7400000000000005E-2</v>
-      </c>
-      <c r="E21" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="B22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.25469999999999998</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.26740000000000003</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.26929999999999998</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B22" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22" t="s">
-        <v>60</v>
-      </c>
-      <c r="D22" s="1">
-        <v>9.5799999999999996E-2</v>
-      </c>
-      <c r="E22" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B23" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" t="s">
-        <v>62</v>
-      </c>
-      <c r="D23" s="1">
-        <v>9.6500000000000002E-2</v>
-      </c>
-      <c r="E23" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B24" t="s">
-        <v>64</v>
-      </c>
-      <c r="C24" t="s">
-        <v>65</v>
-      </c>
-      <c r="D24" s="1">
-        <v>9.6600000000000005E-2</v>
-      </c>
-      <c r="E24" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="C25" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D25" s="1">
-        <v>0.10199999999999999</v>
+        <v>0.35210000000000002</v>
       </c>
       <c r="E25" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="C26" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D26" s="1">
-        <v>0.1101</v>
+        <v>0.44259999999999999</v>
       </c>
       <c r="E26" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="D27" s="1">
         <v>0.112</v>
@@ -1629,15 +1614,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>70</v>
+        <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C28" t="s">
-        <v>71</v>
+        <v>34</v>
       </c>
       <c r="D28" s="1">
         <v>0.1142</v>
@@ -1646,15 +1631,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C29" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="D29" s="1">
         <v>0.12820000000000001</v>
@@ -1663,15 +1648,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C30" t="s">
-        <v>73</v>
+        <v>36</v>
       </c>
       <c r="D30" s="1">
         <v>0.1502</v>
@@ -1680,15 +1665,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C31" t="s">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="D31" s="1">
         <v>0.1762</v>
@@ -1697,15 +1682,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C32" t="s">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="D32" s="1">
         <v>0.23319999999999999</v>
@@ -1714,15 +1699,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C33" t="s">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="D33" s="1">
         <v>0.28539999999999999</v>
@@ -1731,15 +1716,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D34" s="1"/>
       <c r="E34" s="2"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D35" s="1"/>
       <c r="E35" s="2"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D36" s="1"/>
       <c r="E36" s="2"/>
     </row>

</xml_diff>

<commit_message>
ChatGPT for monthly report
</commit_message>
<xml_diff>
--- a/site/res/json/_Last-month-raceData.xlsx
+++ b/site/res/json/_Last-month-raceData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\git\frimleyFlyers\site\res\json\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1FEA2F6-46A3-4C9A-9C33-4E01CD25E7BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B0E80D1-9CA0-4F8B-B596-E85DFE215AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F8E35614-E497-4037-9098-C44996FE8116}"/>
+    <workbookView xWindow="-23340" yWindow="3090" windowWidth="21600" windowHeight="11295" xr2:uid="{F8E35614-E497-4037-9098-C44996FE8116}"/>
   </bookViews>
   <sheets>
     <sheet name="b-raceData2024.json" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="80">
   <si>
     <t>Column1</t>
   </si>
@@ -257,6 +257,9 @@
   </si>
   <si>
     <t xml:space="preserve">34:14	</t>
+  </si>
+  <si>
+    <t>Column12</t>
   </si>
 </sst>
 </file>
@@ -804,7 +807,25 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
@@ -827,16 +848,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C43F3247-6DA4-4454-A121-70C5927A9352}" name="Table1" displayName="Table1" ref="A1:E36" totalsRowShown="0">
-  <autoFilter ref="A1:E36" xr:uid="{C43F3247-6DA4-4454-A121-70C5927A9352}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E36">
-    <sortCondition ref="D3:D36"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C43F3247-6DA4-4454-A121-70C5927A9352}" name="Table1" displayName="Table1" ref="A1:F36" totalsRowShown="0">
+  <autoFilter ref="A1:F36" xr:uid="{C43F3247-6DA4-4454-A121-70C5927A9352}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:F36">
+    <sortCondition ref="E3:E36"/>
   </sortState>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{D3F63264-017A-4E07-B914-C5F98CA77055}" name="Column1" dataDxfId="1"/>
+  <tableColumns count="6">
+    <tableColumn id="6" xr3:uid="{2EE57549-C73C-457E-AC72-DDC94B55CE3B}" name="Column12" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{D3F63264-017A-4E07-B914-C5F98CA77055}" name="Column1" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{741C0D26-66B1-4900-9F9A-207388BA93A5}" name="Column2"/>
     <tableColumn id="3" xr3:uid="{AC85C6D5-0322-45AA-82DD-A19FD0112578}" name="Column3"/>
-    <tableColumn id="4" xr3:uid="{8711641C-9A00-4D46-9C48-CB28E1BCC94B}" name="Column4" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{8711641C-9A00-4D46-9C48-CB28E1BCC94B}" name="Column4" dataDxfId="1"/>
     <tableColumn id="5" xr3:uid="{8727F302-2B57-4FB3-856C-2733213E68D8}" name="Column5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1160,591 +1182,689 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D1D6B08-1595-4967-9FDC-03B96CFA29A2}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
       <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>-0.158</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>38</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>-0.12520000000000001</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
       <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>-6.4000000000000001E-2</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="2">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>41</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>-5.0200000000000002E-2</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
       <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>-4.3200000000000002E-2</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7" s="2">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>31</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>-3.5900000000000001E-2</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
       <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <v>-8.5000000000000006E-3</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F9" s="2">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
       <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="E10" s="2">
+      <c r="F10" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
       <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="1">
+      <c r="E11" s="1">
         <v>1.5699999999999999E-2</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F11" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>49</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="1">
+      <c r="E12" s="1">
         <v>2.0500000000000001E-2</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F12" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>52</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="1">
+      <c r="E13" s="1">
         <v>2.1600000000000001E-2</v>
       </c>
-      <c r="E13" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B14" t="s">
-        <v>20</v>
-      </c>
       <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="1">
+      <c r="E14" s="1">
         <v>2.41E-2</v>
       </c>
-      <c r="E14" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>31</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="1">
+      <c r="E15" s="1">
         <v>2.52E-2</v>
       </c>
-      <c r="E15" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="F15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>49</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="1">
+      <c r="E16" s="1">
         <v>3.85E-2</v>
       </c>
-      <c r="E16" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="F16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>41</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="1">
+      <c r="E17" s="1">
         <v>4.3200000000000002E-2</v>
       </c>
-      <c r="E17" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="F17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B18" t="s">
-        <v>20</v>
-      </c>
       <c r="C18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="1">
+      <c r="E18" s="1">
         <v>6.1499999999999999E-2</v>
       </c>
-      <c r="E18" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="F18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B19" t="s">
-        <v>20</v>
-      </c>
       <c r="C19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="1">
+      <c r="E19" s="1">
         <v>6.2300000000000001E-2</v>
       </c>
-      <c r="E19" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="F19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B20" t="s">
-        <v>20</v>
-      </c>
       <c r="C20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="1">
+      <c r="E20" s="1">
         <v>6.4500000000000002E-2</v>
       </c>
-      <c r="E20" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="F20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>19</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B21" t="s">
-        <v>20</v>
-      </c>
       <c r="C21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" t="s">
         <v>62</v>
       </c>
-      <c r="D21" s="1">
+      <c r="E21" s="1">
         <v>7.3400000000000007E-2</v>
       </c>
-      <c r="E21" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="F21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>20</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B22" t="s">
-        <v>20</v>
-      </c>
       <c r="C22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" t="s">
         <v>63</v>
       </c>
-      <c r="D22" s="1">
+      <c r="E22" s="1">
         <v>8.2199999999999995E-2</v>
       </c>
-      <c r="E22" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="F22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>21</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>64</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>65</v>
       </c>
-      <c r="D23" s="1">
+      <c r="E23" s="1">
         <v>8.7800000000000003E-2</v>
       </c>
-      <c r="E23" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="F23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>22</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>67</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>68</v>
       </c>
-      <c r="D24" s="1">
+      <c r="E24" s="1">
         <v>9.5799999999999996E-2</v>
       </c>
-      <c r="E24" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="F24" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>23</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B25" t="s">
-        <v>20</v>
-      </c>
       <c r="C25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" t="s">
         <v>69</v>
       </c>
-      <c r="D25" s="1">
+      <c r="E25" s="1">
         <v>0.13089999999999999</v>
       </c>
-      <c r="E25" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="F25" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>24</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B26" t="s">
-        <v>20</v>
-      </c>
       <c r="C26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" t="s">
         <v>70</v>
       </c>
-      <c r="D26" s="1">
+      <c r="E26" s="1">
         <v>0.17430000000000001</v>
       </c>
-      <c r="E26" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="F26" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>25</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B27" t="s">
-        <v>20</v>
-      </c>
       <c r="C27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" t="s">
         <v>71</v>
       </c>
-      <c r="D27" s="1">
+      <c r="E27" s="1">
         <v>0.24299999999999999</v>
       </c>
-      <c r="E27" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="F27" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>26</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B28" t="s">
-        <v>20</v>
-      </c>
       <c r="C28" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" t="s">
         <v>73</v>
       </c>
-      <c r="D28" s="1">
+      <c r="E28" s="1">
         <v>0.26479999999999998</v>
       </c>
-      <c r="E28" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="F28" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>27</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B29" t="s">
-        <v>20</v>
-      </c>
       <c r="C29" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" t="s">
         <v>75</v>
       </c>
-      <c r="D29" s="1">
+      <c r="E29" s="1">
         <v>0.32690000000000002</v>
       </c>
-      <c r="E29" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="F29" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>28</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
-        <v>20</v>
-      </c>
       <c r="C30" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" t="s">
         <v>76</v>
       </c>
-      <c r="D30" s="1">
+      <c r="E30" s="1">
         <v>0.35499999999999998</v>
       </c>
-      <c r="E30" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="F30" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>29</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B31" t="s">
-        <v>20</v>
-      </c>
       <c r="C31" t="s">
+        <v>20</v>
+      </c>
+      <c r="D31" t="s">
         <v>78</v>
       </c>
-      <c r="D31" s="1">
+      <c r="E31" s="1">
         <v>0.56910000000000005</v>
       </c>
-      <c r="E31" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="F31" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>30</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B32" t="s">
-        <v>20</v>
-      </c>
       <c r="C32" t="s">
+        <v>20</v>
+      </c>
+      <c r="D32" t="s">
         <v>28</v>
       </c>
-      <c r="D32" s="1">
+      <c r="E32" s="1">
         <v>0.23319999999999999</v>
       </c>
-      <c r="E32" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="F32" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>31</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B33" t="s">
-        <v>20</v>
-      </c>
       <c r="C33" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" t="s">
         <v>30</v>
       </c>
-      <c r="D33" s="1">
+      <c r="E33" s="1">
         <v>0.28539999999999999</v>
       </c>
-      <c r="E33" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D34" s="1"/>
-      <c r="E34" s="2"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D35" s="1"/>
-      <c r="E35" s="2"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D36" s="1"/>
-      <c r="E36" s="2"/>
+      <c r="F33" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E34" s="1"/>
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E35" s="1"/>
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E36" s="1"/>
+      <c r="F36" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>

</xml_diff>